<commit_message>
Maj Cell_Arr : Tube Suspension
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\Frame_Analysis\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\True_Frame_Analysis\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6ABBBE-11C4-43A8-8158-A976AC38F935}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770AEA06-FE77-4A37-8422-8A6ABDD58203}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{A823F9F4-64D6-48B0-A8D5-F67E22E275E5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Calcul de rigidité</t>
   </si>
@@ -68,6 +68,45 @@
   </si>
   <si>
     <t>Front/Rear</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Largeur</t>
+  </si>
+  <si>
+    <t>Couple</t>
+  </si>
+  <si>
+    <t>Deplacement en Z</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Rear</t>
+  </si>
+  <si>
+    <t>Upper A-Arm Front</t>
+  </si>
+  <si>
+    <t>Upper A-Arm Rear</t>
+  </si>
+  <si>
+    <t>Lower A-Arm Front</t>
+  </si>
+  <si>
+    <t>Lower A-Arm Rear</t>
+  </si>
+  <si>
+    <t>Déplacement en X</t>
   </si>
 </sst>
 </file>
@@ -130,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -143,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,14 +519,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -624,32 +666,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C38C1A-568D-4F7A-B16B-E2DE231D017C}">
-  <dimension ref="B2:L16"/>
+  <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="11.5546875" style="1"/>
+    <col min="7" max="7" width="26.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.5546875" style="1"/>
     <col min="12" max="12" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
       <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
@@ -670,21 +718,26 @@
       <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="2">
         <v>227</v>
       </c>
@@ -697,7 +750,12 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -706,7 +764,12 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -715,7 +778,12 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -724,7 +792,12 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -733,7 +806,12 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -742,7 +820,12 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -751,7 +834,12 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -786,6 +874,57 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.22700000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1">
+        <f>H22*H23</f>
+        <v>181.6</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="1">
+        <f>H25/H23</f>
+        <v>1.3215859030837005E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="1">
+        <f>H24/H26</f>
+        <v>13741.066666666666</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E2:F3"/>

</xml_diff>

<commit_message>
Cas de charges Frame
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\True_Frame_Analysis\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770AEA06-FE77-4A37-8422-8A6ABDD58203}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28A1483-0AB1-43F6-ABF3-CDFB120C0389}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{A823F9F4-64D6-48B0-A8D5-F67E22E275E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A823F9F4-64D6-48B0-A8D5-F67E22E275E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1 (2)" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Calcul de rigidité</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Front/Rear</t>
-  </si>
-  <si>
-    <t>Force</t>
   </si>
   <si>
     <t>Largeur</t>
@@ -169,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,6 +184,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C38C1A-568D-4F7A-B16B-E2DE231D017C}">
-  <dimension ref="B2:L27"/>
+  <dimension ref="A2:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,17 +687,18 @@
     <col min="9" max="9" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.5546875" style="1"/>
     <col min="12" max="12" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="1"/>
+    <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>
@@ -702,7 +706,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P4" s="1">
+        <f>2*1000*0.219</f>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -719,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>4</v>
@@ -731,12 +741,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2">
         <v>227</v>
@@ -748,13 +758,16 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="Q6" s="1">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -762,13 +775,28 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="1">
+        <f>620/L9</f>
+        <v>425.37956139696814</v>
+      </c>
+      <c r="M7" s="1">
+        <f>1281/L7</f>
+        <v>3.011428183792213</v>
+      </c>
+      <c r="O7" s="1">
+        <f>L7*M7</f>
+        <v>1281</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -776,13 +804,21 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="1">
+        <f>PI()/180</f>
+        <v>1.7453292519943295E-2</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>ATAN((Q6+Q7)/0.438)</f>
+        <v>5.7015762900504474E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -790,13 +826,21 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L9" s="1">
+        <f>ATAN((2.73+2.72)/0.62)</f>
+        <v>1.4575218375887371</v>
+      </c>
+      <c r="M9" s="1">
+        <f>180/PI()</f>
+        <v>57.295779513082323</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -805,12 +849,12 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -818,13 +862,17 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="P11" s="1">
+        <f>P4/Q8</f>
+        <v>7682.0861059832387</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -833,12 +881,12 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -847,7 +895,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -856,7 +904,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -865,7 +913,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -874,55 +922,102 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F22" s="1" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <f>0.227*2+0.6</f>
+        <v>1.054</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.219</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>720</v>
+      </c>
+      <c r="B22" s="1">
+        <f>ATAN((0.00183+0.00051)/1)</f>
+        <v>2.3399957290460315E-3</v>
+      </c>
+      <c r="K22" s="1">
+        <f>800*K21</f>
+        <v>843.2</v>
+      </c>
+      <c r="M22" s="7">
+        <f>M21*1000</f>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <f>A22/(180*B22)</f>
+        <v>1709.4048293971537</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="1">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K23" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="1">
-        <v>0.22700000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1">
+        <v>720</v>
+      </c>
+      <c r="K24" s="1">
+        <f>ATAN(K23/K21)</f>
+        <v>4.2694237741913929E-3</v>
+      </c>
+      <c r="M24" s="1">
+        <f>ATAN(0.00292/0.438)*180</f>
+        <v>1.1999822226962811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H24" s="1">
-        <f>H22*H23</f>
-        <v>181.6</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F25" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="H25" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <f>K22/(K24*180)</f>
+        <v>1097.2076542885825</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" s="1">
         <f>H25/H23</f>
-        <v>1.3215859030837005E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.3">
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="I26" s="1">
+        <f>H26*180</f>
+        <v>0.6</v>
+      </c>
+      <c r="M26" s="8">
+        <f>M22/M24</f>
+        <v>182.50270367166058</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="1">
-        <f>H24/H26</f>
-        <v>13741.066666666666</v>
+        <f>H24/(H26*180)</f>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -930,5 +1025,6 @@
     <mergeCell ref="E2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Simu MAXSPEED rigidité châssis
Rectification de la simulation Maxspeed
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\True_Frame_Analysis\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9317D4F-C09A-4F00-84BF-F48D2571E58B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Right Turn 2,2G" sheetId="6" r:id="rId6"/>
     <sheet name="MAX SPEED" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -81,13 +75,13 @@
     <t>Appliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en y</t>
   </si>
   <si>
-    <t>Appliquer les mêmes effoAppliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en yrts de la roue droite sur la roue gauche</t>
+    <t>Appliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en yrts de la roue droite sur la roue gauche</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +281,7 @@
         <xdr:cNvPr id="2" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -358,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,26 +385,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,23 +420,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK21"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
@@ -897,7 +857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1052,7 +1012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1267,7 +1227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1422,7 +1382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1575,7 +1535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1728,11 +1688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1748,17 +1708,17 @@
     <col min="11" max="1025" width="11.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1775,150 +1735,150 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="6">
         <v>1</v>
       </c>
       <c r="D6" s="6">
-        <v>-7.7899999999999997E-2</v>
+        <v>-8.6699999999999999E-2</v>
       </c>
       <c r="E6" s="6">
-        <v>0.11600000000000001</v>
+        <v>-3.5500000000000002E-3</v>
       </c>
       <c r="F6" s="6">
-        <v>5.72</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="6">
         <v>2</v>
       </c>
       <c r="D7" s="6">
-        <v>-5.1299999999999998E-2</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="E7" s="6">
-        <v>0.11600000000000001</v>
+        <v>-4.7999999999999996E-3</v>
       </c>
       <c r="F7" s="6">
-        <v>5.57</v>
-      </c>
-      <c r="I7" s="1" t="s">
+        <v>5.35</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="6">
         <v>3</v>
       </c>
       <c r="D8" s="6">
-        <v>-7.7499999999999999E-2</v>
+        <v>-5.6399999999999999E-2</v>
       </c>
       <c r="E8" s="6">
-        <v>8.1299999999999997E-2</v>
+        <v>-1.92E-4</v>
       </c>
       <c r="F8" s="6">
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>4</v>
       </c>
       <c r="D9" s="6">
-        <v>-5.3100000000000001E-2</v>
+        <v>-5.62E-2</v>
       </c>
       <c r="E9" s="6">
-        <v>7.8799999999999995E-2</v>
+        <v>-1.6900000000000001E-3</v>
       </c>
       <c r="F9" s="6">
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="6">
         <v>5</v>
       </c>
       <c r="D10" s="6">
-        <v>-7.8299999999999995E-2</v>
+        <v>-8.9599999999999999E-2</v>
       </c>
       <c r="E10" s="6">
-        <v>5.5599999999999997E-2</v>
+        <v>1.04E-2</v>
       </c>
       <c r="F10" s="6">
-        <v>3.38</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="6">
         <v>6</v>
       </c>
       <c r="D11" s="6">
-        <v>-5.45E-2</v>
+        <v>-5.8900000000000001E-2</v>
       </c>
       <c r="E11" s="6">
-        <v>5.7799999999999997E-2</v>
+        <v>1.2099999999999999E-3</v>
       </c>
       <c r="F11" s="6">
-        <v>3.28</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="6">
         <v>7</v>
       </c>
       <c r="D12" s="6">
-        <v>0.10299999999999999</v>
+        <v>0.107</v>
       </c>
       <c r="E12" s="6">
-        <v>3.2300000000000002E-2</v>
+        <v>-3.2000000000000003E-4</v>
       </c>
       <c r="F12" s="6">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="6">
         <v>8</v>
       </c>
       <c r="D13" s="6">
-        <v>0.128</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E13" s="6">
-        <v>3.9300000000000002E-2</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="F13" s="6">
-        <v>1.24</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="6">
         <v>9</v>
       </c>
       <c r="D14" s="6">
-        <v>1.78E-2</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="E14" s="6">
-        <v>2.3800000000000002E-2</v>
+        <v>2.35E-2</v>
       </c>
       <c r="F14" s="6">
-        <v>0.60299999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="6">
         <v>10</v>
       </c>
       <c r="D15" s="6">
-        <v>3.7999999999999999E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="E15" s="6">
-        <v>1.9900000000000001E-2</v>
+        <v>-1.08E-3</v>
       </c>
       <c r="F15" s="6">
-        <v>0.60399999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>

</xml_diff>

<commit_message>
Simu bump3g rigidité châssis
Ajout de la simulation bump3g de la rigidité du châssis
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
         <xdr:cNvPr id="2" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,17 +1278,29 @@
       <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="6">
+        <v>-0.25600000000000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>-9.1699999999999993E-3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="6">
+        <v>-0.158</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.35E-2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>15</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1297,65 +1309,114 @@
       <c r="C8" s="6">
         <v>3</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="6">
+        <v>-0.158</v>
+      </c>
+      <c r="E8" s="6">
+        <f>2.72*10^-6</f>
+        <v>2.7200000000000002E-6</v>
+      </c>
+      <c r="F8" s="6">
+        <v>12.3</v>
+      </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>4</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="6">
+        <v>-0.157</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-5.2599999999999999E-3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>12.3</v>
+      </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="6">
         <v>5</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="6">
+        <v>-0.161</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-7.4099999999999999E-3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8.91</v>
+      </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="6">
         <v>6</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="D11" s="6">
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.74E-3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8.91</v>
+      </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="6">
         <v>7</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="6">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-1.46E-2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3.32</v>
+      </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="6">
         <v>8</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="D13" s="6">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3.34</v>
+      </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="6">
         <v>9</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="6">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1.61</v>
+      </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C15" s="6">
         <v>10</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="6">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-2.81E-3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1.61</v>
+      </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
@@ -1691,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Simu Right turn 2,2g rigidité châssis
Ajout des Simu right turn 2,2g pour la rigidité du châssis
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Analyse - Cas de Charges Frame</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Appliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en yrts de la roue droite sur la roue gauche</t>
+  </si>
+  <si>
+    <t>Right Turn 2,2G</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
         <xdr:cNvPr id="2" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1599,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" activeCellId="1" sqref="D6:F15 C15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1620,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.3">
@@ -1645,17 +1650,29 @@
       <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="6">
+        <v>-0.60499999999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <v>637</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="6">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6.37</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5.84</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1664,65 +1681,113 @@
       <c r="C8" s="6">
         <v>3</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="6">
+        <v>-0.58599999999999997</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5.45</v>
+      </c>
+      <c r="F8" s="6">
+        <v>4.33</v>
+      </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>4</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="6">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5.44</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4.78</v>
+      </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="6">
         <v>5</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="6">
+        <v>-0.58799999999999997</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="F10" s="6">
+        <v>3.01</v>
+      </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="6">
         <v>6</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="D11" s="6">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4.41</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3.58</v>
+      </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="6">
         <v>7</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="6">
+        <v>-0.41899999999999998</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2.15</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.91600000000000004</v>
+      </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="6">
         <v>8</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="D13" s="6">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2.13</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1.55</v>
+      </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="6">
         <v>9</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="6">
+        <v>-0.39200000000000002</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="F14" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C15" s="6">
         <v>10</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.38</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.90300000000000002</v>
+      </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
@@ -1753,7 +1818,7 @@
   <dimension ref="A2:AMK26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cas de charge chassis left turn 2,2G
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/True_Frame_Analysis/Results/Invictus_rigidité.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Braking 1,9G" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Bump_3G" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Left Turn 2,2G" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Right Turn 2,2G" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="MAX SPEED" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="MAX SPEED" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Right Turn 2,2G" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -64,16 +64,16 @@
     <t xml:space="preserve">Mettre comme effort sur la roue gauche, les forces symétriques par rapport au plan (x,y), du cas Right Turn 2,2G</t>
   </si>
   <si>
+    <t xml:space="preserve">MAX SPEED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en yrts de la roue droite sur la roue gauche</t>
+  </si>
+  <si>
     <t xml:space="preserve">Right Turn 2,2G</t>
   </si>
   <si>
     <t xml:space="preserve">Mettre comme effort sur la roue gauche, les forces symétriques par rapport au plan (x,y), du cas Left Turn 2,2G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX SPEED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appliquer les mêmes efforts de la roue droite sur la roue gauche, en inversant la valeur en yrts de la roue droite sur la roue gauche</t>
   </si>
 </sst>
 </file>
@@ -299,9 +299,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -315,7 +315,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1693800"/>
-          <a:ext cx="6177240" cy="3090960"/>
+          <a:ext cx="6177960" cy="3090600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -343,11 +343,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,21 +607,21 @@
   </sheetPr>
   <dimension ref="C2:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,15 +833,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,15 +1053,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,21 +1268,21 @@
   </sheetPr>
   <dimension ref="C2:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,17 +1314,29 @@
       <c r="C6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="D6" s="8" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>-2.39</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>-2.9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="D7" s="8" t="n">
+        <v>-0.183</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>-2.39</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>-2.15</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1333,65 +1345,113 @@
       <c r="C8" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="D8" s="8" t="n">
+        <v>0.258</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>-1.91</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>-2.4</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="8" t="n">
+        <v>-0.166</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>-1.92</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>-1.78</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="8" t="n">
+        <v>0.243</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>-1.89</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="8" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>-1.52</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>-1.39</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="D12" s="8" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>-0.768</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>-0.662</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="8" t="n">
+        <v>-0.233</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>-0.77</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>-0.686</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="8" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>-0.494</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="D15" s="8" t="n">
+        <v>-0.138</v>
+      </c>
+      <c r="E15" s="8" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>-0.385</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="8"/>
@@ -1427,20 +1487,20 @@
   <dimension ref="C2:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,13 +1535,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="n">
-        <v>-0.605</v>
+        <v>-0.0867</v>
       </c>
       <c r="E6" s="8" t="n">
-        <v>637</v>
+        <v>-0.00355</v>
       </c>
       <c r="F6" s="8" t="n">
-        <v>5.27</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,15 +1549,15 @@
         <v>2</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>0.461</v>
+        <v>-0.055</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>6.37</v>
+        <v>-0.0048</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>5.84</v>
-      </c>
-      <c r="I7" s="1" t="s">
+        <v>5.35</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1506,13 +1566,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="8" t="n">
-        <v>-0.586</v>
+        <v>-0.0564</v>
       </c>
       <c r="E8" s="8" t="n">
-        <v>5.45</v>
+        <v>-0.000192</v>
       </c>
       <c r="F8" s="8" t="n">
-        <v>4.33</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,13 +1580,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0.474</v>
+        <v>-0.0562</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>5.44</v>
+        <v>-0.00169</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>4.78</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,13 +1594,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="8" t="n">
-        <v>-0.588</v>
+        <v>-0.0896</v>
       </c>
       <c r="E10" s="8" t="n">
-        <v>4.39</v>
+        <v>0.0104</v>
       </c>
       <c r="F10" s="8" t="n">
-        <v>3.01</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,13 +1608,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>0.445</v>
+        <v>-0.0589</v>
       </c>
       <c r="E11" s="8" t="n">
-        <v>4.41</v>
+        <v>0.00121</v>
       </c>
       <c r="F11" s="8" t="n">
-        <v>3.58</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,13 +1622,13 @@
         <v>7</v>
       </c>
       <c r="D12" s="8" t="n">
-        <v>-0.419</v>
+        <v>0.107</v>
       </c>
       <c r="E12" s="8" t="n">
-        <v>2.15</v>
+        <v>-0.00032</v>
       </c>
       <c r="F12" s="8" t="n">
-        <v>0.916</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,13 +1636,13 @@
         <v>8</v>
       </c>
       <c r="D13" s="8" t="n">
-        <v>0.636</v>
+        <v>0.018</v>
       </c>
       <c r="E13" s="8" t="n">
-        <v>2.13</v>
+        <v>0.0056</v>
       </c>
       <c r="F13" s="8" t="n">
-        <v>1.55</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,13 +1650,13 @@
         <v>9</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>-0.392</v>
+        <v>-0.016</v>
       </c>
       <c r="E14" s="8" t="n">
-        <v>1.42</v>
+        <v>0.0235</v>
       </c>
       <c r="F14" s="8" t="n">
-        <v>0.035</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,13 +1664,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0.382</v>
+        <v>0.0325</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>1.38</v>
+        <v>-0.00108</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>0.903</v>
+        <v>0.576</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,20 +1707,20 @@
   <dimension ref="C2:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,13 +1755,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="n">
-        <v>-0.0867</v>
+        <v>-0.605</v>
       </c>
       <c r="E6" s="8" t="n">
-        <v>-0.00355</v>
+        <v>637</v>
       </c>
       <c r="F6" s="8" t="n">
-        <v>5.36</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,15 +1769,15 @@
         <v>2</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>-0.055</v>
+        <v>0.461</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>-0.0048</v>
+        <v>6.37</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="J7" s="1" t="s">
+        <v>5.84</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1726,13 +1786,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="8" t="n">
-        <v>-0.0564</v>
+        <v>-0.586</v>
       </c>
       <c r="E8" s="8" t="n">
-        <v>-0.000192</v>
+        <v>5.45</v>
       </c>
       <c r="F8" s="8" t="n">
-        <v>4.41</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,13 +1800,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>-0.0562</v>
+        <v>0.474</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>-0.00169</v>
+        <v>5.44</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>4.41</v>
+        <v>4.78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,13 +1814,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="8" t="n">
-        <v>-0.0896</v>
+        <v>-0.588</v>
       </c>
       <c r="E10" s="8" t="n">
-        <v>0.0104</v>
+        <v>4.39</v>
       </c>
       <c r="F10" s="8" t="n">
-        <v>3.17</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,13 +1828,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>-0.0589</v>
+        <v>0.445</v>
       </c>
       <c r="E11" s="8" t="n">
-        <v>0.00121</v>
+        <v>4.41</v>
       </c>
       <c r="F11" s="8" t="n">
-        <v>3.2</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,13 +1842,13 @@
         <v>7</v>
       </c>
       <c r="D12" s="8" t="n">
-        <v>0.107</v>
+        <v>-0.419</v>
       </c>
       <c r="E12" s="8" t="n">
-        <v>-0.00032</v>
+        <v>2.15</v>
       </c>
       <c r="F12" s="8" t="n">
-        <v>1.2</v>
+        <v>0.916</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,13 +1856,13 @@
         <v>8</v>
       </c>
       <c r="D13" s="8" t="n">
-        <v>0.018</v>
+        <v>0.636</v>
       </c>
       <c r="E13" s="8" t="n">
-        <v>0.0056</v>
+        <v>2.13</v>
       </c>
       <c r="F13" s="8" t="n">
-        <v>1.2</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,13 +1870,13 @@
         <v>9</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>-0.016</v>
+        <v>-0.392</v>
       </c>
       <c r="E14" s="8" t="n">
-        <v>0.0235</v>
+        <v>1.42</v>
       </c>
       <c r="F14" s="8" t="n">
-        <v>0.064</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,13 +1884,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0.0325</v>
+        <v>0.382</v>
       </c>
       <c r="E15" s="8" t="n">
-        <v>-0.00108</v>
+        <v>1.38</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>0.576</v>
+        <v>0.903</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>